<commit_message>
add top 10 and 20 analysis results
</commit_message>
<xml_diff>
--- a/StockAssessment/top10_analysis.xlsx
+++ b/StockAssessment/top10_analysis.xlsx
@@ -76,10 +76,10 @@
     <t>wanted catch</t>
   </si>
   <si>
-    <t>forecast</t>
+    <t>projection</t>
   </si>
   <si>
-    <t>projection</t>
+    <t>forecast</t>
   </si>
   <si>
     <t>prediction</t>
@@ -602,10 +602,10 @@
         <v>0.0</v>
       </c>
       <c r="U2" t="n">
-        <v>0.0</v>
+        <v>9.0</v>
       </c>
       <c r="V2" t="n">
-        <v>9.0</v>
+        <v>0.0</v>
       </c>
       <c r="W2" t="n">
         <v>0.0</v>
@@ -706,10 +706,10 @@
         <v>0.0</v>
       </c>
       <c r="U3" t="n">
-        <v>0.0</v>
+        <v>5.0</v>
       </c>
       <c r="V3" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
       <c r="W3" t="n">
         <v>1.0</v>
@@ -1122,10 +1122,10 @@
         <v>0.0</v>
       </c>
       <c r="U7" t="n">
-        <v>0.0</v>
+        <v>8.0</v>
       </c>
       <c r="V7" t="n">
-        <v>8.0</v>
+        <v>0.0</v>
       </c>
       <c r="W7" t="n">
         <v>0.0</v>
@@ -1226,10 +1226,10 @@
         <v>0.0</v>
       </c>
       <c r="U8" t="n">
-        <v>1.0</v>
+        <v>4.0</v>
       </c>
       <c r="V8" t="n">
-        <v>4.0</v>
+        <v>1.0</v>
       </c>
       <c r="W8" t="n">
         <v>13.0</v>
@@ -1330,10 +1330,10 @@
         <v>0.0</v>
       </c>
       <c r="U9" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="V9" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="W9" t="n">
         <v>1.0</v>
@@ -1434,10 +1434,10 @@
         <v>0.0</v>
       </c>
       <c r="U10" t="n">
-        <v>0.0</v>
+        <v>4.0</v>
       </c>
       <c r="V10" t="n">
-        <v>4.0</v>
+        <v>0.0</v>
       </c>
       <c r="W10" t="n">
         <v>0.0</v>
@@ -1538,10 +1538,10 @@
         <v>0.0</v>
       </c>
       <c r="U11" t="n">
-        <v>0.0</v>
+        <v>12.0</v>
       </c>
       <c r="V11" t="n">
-        <v>12.0</v>
+        <v>0.0</v>
       </c>
       <c r="W11" t="n">
         <v>2.0</v>
@@ -1642,10 +1642,10 @@
         <v>0.0</v>
       </c>
       <c r="U12" t="n">
-        <v>0.0</v>
+        <v>9.0</v>
       </c>
       <c r="V12" t="n">
-        <v>9.0</v>
+        <v>0.0</v>
       </c>
       <c r="W12" t="n">
         <v>2.0</v>
@@ -1746,10 +1746,10 @@
         <v>0.0</v>
       </c>
       <c r="U13" t="n">
-        <v>0.0</v>
+        <v>3.0</v>
       </c>
       <c r="V13" t="n">
-        <v>3.0</v>
+        <v>0.0</v>
       </c>
       <c r="W13" t="n">
         <v>0.0</v>
@@ -2058,10 +2058,10 @@
         <v>0.0</v>
       </c>
       <c r="U16" t="n">
-        <v>0.0</v>
+        <v>23.0</v>
       </c>
       <c r="V16" t="n">
-        <v>23.0</v>
+        <v>0.0</v>
       </c>
       <c r="W16" t="n">
         <v>1.0</v>
@@ -2474,10 +2474,10 @@
         <v>0.0</v>
       </c>
       <c r="U20" t="n">
-        <v>0.0</v>
+        <v>6.0</v>
       </c>
       <c r="V20" t="n">
-        <v>6.0</v>
+        <v>0.0</v>
       </c>
       <c r="W20" t="n">
         <v>0.0</v>
@@ -2994,10 +2994,10 @@
         <v>0.0</v>
       </c>
       <c r="U25" t="n">
-        <v>0.0</v>
+        <v>3.0</v>
       </c>
       <c r="V25" t="n">
-        <v>3.0</v>
+        <v>0.0</v>
       </c>
       <c r="W25" t="n">
         <v>0.0</v>
@@ -3098,10 +3098,10 @@
         <v>0.0</v>
       </c>
       <c r="U26" t="n">
-        <v>0.0</v>
+        <v>5.0</v>
       </c>
       <c r="V26" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
       <c r="W26" t="n">
         <v>0.0</v>
@@ -3306,10 +3306,10 @@
         <v>0.0</v>
       </c>
       <c r="U28" t="n">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
       <c r="V28" t="n">
-        <v>2.0</v>
+        <v>0.0</v>
       </c>
       <c r="W28" t="n">
         <v>0.0</v>
@@ -3410,10 +3410,10 @@
         <v>0.0</v>
       </c>
       <c r="U29" t="n">
-        <v>0.0</v>
+        <v>5.0</v>
       </c>
       <c r="V29" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
       <c r="W29" t="n">
         <v>0.0</v>
@@ -3514,10 +3514,10 @@
         <v>0.0</v>
       </c>
       <c r="U30" t="n">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
       <c r="V30" t="n">
-        <v>2.0</v>
+        <v>0.0</v>
       </c>
       <c r="W30" t="n">
         <v>0.0</v>
@@ -3618,10 +3618,10 @@
         <v>0.0</v>
       </c>
       <c r="U31" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="V31" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="W31" t="n">
         <v>0.0</v>
@@ -4034,10 +4034,10 @@
         <v>0.0</v>
       </c>
       <c r="U35" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="V35" t="n">
         <v>29.0</v>
-      </c>
-      <c r="V35" t="n">
-        <v>0.0</v>
       </c>
       <c r="W35" t="n">
         <v>1.0</v>
@@ -4138,10 +4138,10 @@
         <v>0.0</v>
       </c>
       <c r="U36" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="V36" t="n">
         <v>3.0</v>
-      </c>
-      <c r="V36" t="n">
-        <v>2.0</v>
       </c>
       <c r="W36" t="n">
         <v>0.0</v>
@@ -4242,10 +4242,10 @@
         <v>0.0</v>
       </c>
       <c r="U37" t="n">
+        <v>13.0</v>
+      </c>
+      <c r="V37" t="n">
         <v>11.0</v>
-      </c>
-      <c r="V37" t="n">
-        <v>13.0</v>
       </c>
       <c r="W37" t="n">
         <v>8.0</v>
@@ -4346,10 +4346,10 @@
         <v>0.0</v>
       </c>
       <c r="U38" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="V38" t="n">
         <v>4.0</v>
-      </c>
-      <c r="V38" t="n">
-        <v>3.0</v>
       </c>
       <c r="W38" t="n">
         <v>0.0</v>
@@ -4450,10 +4450,10 @@
         <v>0.0</v>
       </c>
       <c r="U39" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="V39" t="n">
         <v>8.0</v>
-      </c>
-      <c r="V39" t="n">
-        <v>0.0</v>
       </c>
       <c r="W39" t="n">
         <v>0.0</v>
@@ -4554,10 +4554,10 @@
         <v>0.0</v>
       </c>
       <c r="U40" t="n">
+        <v>14.0</v>
+      </c>
+      <c r="V40" t="n">
         <v>9.0</v>
-      </c>
-      <c r="V40" t="n">
-        <v>14.0</v>
       </c>
       <c r="W40" t="n">
         <v>4.0</v>
@@ -4658,10 +4658,10 @@
         <v>0.0</v>
       </c>
       <c r="U41" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="V41" t="n">
         <v>10.0</v>
-      </c>
-      <c r="V41" t="n">
-        <v>3.0</v>
       </c>
       <c r="W41" t="n">
         <v>0.0</v>
@@ -4762,10 +4762,10 @@
         <v>0.0</v>
       </c>
       <c r="U42" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="V42" t="n">
         <v>10.0</v>
-      </c>
-      <c r="V42" t="n">
-        <v>6.0</v>
       </c>
       <c r="W42" t="n">
         <v>0.0</v>
@@ -4970,10 +4970,10 @@
         <v>0.0</v>
       </c>
       <c r="U44" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="V44" t="n">
         <v>4.0</v>
-      </c>
-      <c r="V44" t="n">
-        <v>0.0</v>
       </c>
       <c r="W44" t="n">
         <v>0.0</v>
@@ -5074,10 +5074,10 @@
         <v>0.0</v>
       </c>
       <c r="U45" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="V45" t="n">
         <v>48.0</v>
-      </c>
-      <c r="V45" t="n">
-        <v>5.0</v>
       </c>
       <c r="W45" t="n">
         <v>0.0</v>
@@ -5282,10 +5282,10 @@
         <v>0.0</v>
       </c>
       <c r="U47" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="V47" t="n">
         <v>5.0</v>
-      </c>
-      <c r="V47" t="n">
-        <v>2.0</v>
       </c>
       <c r="W47" t="n">
         <v>0.0</v>
@@ -5386,10 +5386,10 @@
         <v>0.0</v>
       </c>
       <c r="U48" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="V48" t="n">
         <v>7.0</v>
-      </c>
-      <c r="V48" t="n">
-        <v>5.0</v>
       </c>
       <c r="W48" t="n">
         <v>7.0</v>
@@ -5490,10 +5490,10 @@
         <v>0.0</v>
       </c>
       <c r="U49" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="V49" t="n">
         <v>21.0</v>
-      </c>
-      <c r="V49" t="n">
-        <v>4.0</v>
       </c>
       <c r="W49" t="n">
         <v>5.0</v>
@@ -5594,10 +5594,10 @@
         <v>0.0</v>
       </c>
       <c r="U50" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="V50" t="n">
         <v>2.0</v>
-      </c>
-      <c r="V50" t="n">
-        <v>0.0</v>
       </c>
       <c r="W50" t="n">
         <v>0.0</v>
@@ -5698,10 +5698,10 @@
         <v>0.0</v>
       </c>
       <c r="U51" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="V51" t="n">
         <v>10.0</v>
-      </c>
-      <c r="V51" t="n">
-        <v>2.0</v>
       </c>
       <c r="W51" t="n">
         <v>0.0</v>
@@ -5906,10 +5906,10 @@
         <v>0.0</v>
       </c>
       <c r="U53" t="n">
-        <v>0.0</v>
+        <v>12.0</v>
       </c>
       <c r="V53" t="n">
-        <v>12.0</v>
+        <v>0.0</v>
       </c>
       <c r="W53" t="n">
         <v>0.0</v>
@@ -6114,10 +6114,10 @@
         <v>0.0</v>
       </c>
       <c r="U55" t="n">
-        <v>0.0</v>
+        <v>25.0</v>
       </c>
       <c r="V55" t="n">
-        <v>25.0</v>
+        <v>0.0</v>
       </c>
       <c r="W55" t="n">
         <v>0.0</v>
@@ -6426,10 +6426,10 @@
         <v>0.0</v>
       </c>
       <c r="U58" t="n">
-        <v>0.0</v>
+        <v>5.0</v>
       </c>
       <c r="V58" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
       <c r="W58" t="n">
         <v>0.0</v>
@@ -6738,10 +6738,10 @@
         <v>0.0</v>
       </c>
       <c r="U61" t="n">
-        <v>0.0</v>
+        <v>3.0</v>
       </c>
       <c r="V61" t="n">
-        <v>3.0</v>
+        <v>0.0</v>
       </c>
       <c r="W61" t="n">
         <v>0.0</v>
@@ -6842,10 +6842,10 @@
         <v>0.0</v>
       </c>
       <c r="U62" t="n">
-        <v>0.0</v>
+        <v>6.0</v>
       </c>
       <c r="V62" t="n">
-        <v>6.0</v>
+        <v>0.0</v>
       </c>
       <c r="W62" t="n">
         <v>0.0</v>
@@ -6946,10 +6946,10 @@
         <v>0.0</v>
       </c>
       <c r="U63" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="V63" t="n">
         <v>3.0</v>
-      </c>
-      <c r="V63" t="n">
-        <v>6.0</v>
       </c>
       <c r="W63" t="n">
         <v>4.0</v>
@@ -7050,10 +7050,10 @@
         <v>0.0</v>
       </c>
       <c r="U64" t="n">
-        <v>0.0</v>
+        <v>4.0</v>
       </c>
       <c r="V64" t="n">
-        <v>4.0</v>
+        <v>0.0</v>
       </c>
       <c r="W64" t="n">
         <v>0.0</v>
@@ -7154,10 +7154,10 @@
         <v>0.0</v>
       </c>
       <c r="U65" t="n">
-        <v>0.0</v>
+        <v>38.0</v>
       </c>
       <c r="V65" t="n">
-        <v>38.0</v>
+        <v>0.0</v>
       </c>
       <c r="W65" t="n">
         <v>3.0</v>
@@ -7258,10 +7258,10 @@
         <v>0.0</v>
       </c>
       <c r="U66" t="n">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
       <c r="V66" t="n">
-        <v>2.0</v>
+        <v>0.0</v>
       </c>
       <c r="W66" t="n">
         <v>0.0</v>
@@ -7362,10 +7362,10 @@
         <v>0.0</v>
       </c>
       <c r="U67" t="n">
-        <v>0.0</v>
+        <v>6.0</v>
       </c>
       <c r="V67" t="n">
-        <v>6.0</v>
+        <v>0.0</v>
       </c>
       <c r="W67" t="n">
         <v>0.0</v>
@@ -7570,10 +7570,10 @@
         <v>0.0</v>
       </c>
       <c r="U69" t="n">
-        <v>0.0</v>
+        <v>43.0</v>
       </c>
       <c r="V69" t="n">
-        <v>43.0</v>
+        <v>0.0</v>
       </c>
       <c r="W69" t="n">
         <v>2.0</v>
@@ -7674,10 +7674,10 @@
         <v>0.0</v>
       </c>
       <c r="U70" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="V70" t="n">
         <v>2.0</v>
-      </c>
-      <c r="V70" t="n">
-        <v>6.0</v>
       </c>
       <c r="W70" t="n">
         <v>0.0</v>
@@ -7778,10 +7778,10 @@
         <v>0.0</v>
       </c>
       <c r="U71" t="n">
-        <v>0.0</v>
+        <v>109.0</v>
       </c>
       <c r="V71" t="n">
-        <v>109.0</v>
+        <v>0.0</v>
       </c>
       <c r="W71" t="n">
         <v>2.0</v>
@@ -7882,10 +7882,10 @@
         <v>0.0</v>
       </c>
       <c r="U72" t="n">
+        <v>25.0</v>
+      </c>
+      <c r="V72" t="n">
         <v>3.0</v>
-      </c>
-      <c r="V72" t="n">
-        <v>25.0</v>
       </c>
       <c r="W72" t="n">
         <v>1.0</v>
@@ -7986,10 +7986,10 @@
         <v>0.0</v>
       </c>
       <c r="U73" t="n">
+        <v>17.0</v>
+      </c>
+      <c r="V73" t="n">
         <v>7.0</v>
-      </c>
-      <c r="V73" t="n">
-        <v>17.0</v>
       </c>
       <c r="W73" t="n">
         <v>1.0</v>
@@ -8090,10 +8090,10 @@
         <v>0.0</v>
       </c>
       <c r="U74" t="n">
-        <v>0.0</v>
+        <v>8.0</v>
       </c>
       <c r="V74" t="n">
-        <v>8.0</v>
+        <v>0.0</v>
       </c>
       <c r="W74" t="n">
         <v>1.0</v>
@@ -8194,10 +8194,10 @@
         <v>0.0</v>
       </c>
       <c r="U75" t="n">
+        <v>17.0</v>
+      </c>
+      <c r="V75" t="n">
         <v>2.0</v>
-      </c>
-      <c r="V75" t="n">
-        <v>17.0</v>
       </c>
       <c r="W75" t="n">
         <v>4.0</v>
@@ -8298,10 +8298,10 @@
         <v>0.0</v>
       </c>
       <c r="U76" t="n">
+        <v>16.0</v>
+      </c>
+      <c r="V76" t="n">
         <v>18.0</v>
-      </c>
-      <c r="V76" t="n">
-        <v>16.0</v>
       </c>
       <c r="W76" t="n">
         <v>1.0</v>
@@ -8402,10 +8402,10 @@
         <v>0.0</v>
       </c>
       <c r="U77" t="n">
-        <v>1.0</v>
+        <v>13.0</v>
       </c>
       <c r="V77" t="n">
-        <v>13.0</v>
+        <v>1.0</v>
       </c>
       <c r="W77" t="n">
         <v>1.0</v>
@@ -8506,10 +8506,10 @@
         <v>0.0</v>
       </c>
       <c r="U78" t="n">
-        <v>0.0</v>
+        <v>37.0</v>
       </c>
       <c r="V78" t="n">
-        <v>37.0</v>
+        <v>0.0</v>
       </c>
       <c r="W78" t="n">
         <v>2.0</v>
@@ -8610,10 +8610,10 @@
         <v>0.0</v>
       </c>
       <c r="U79" t="n">
-        <v>0.0</v>
+        <v>42.0</v>
       </c>
       <c r="V79" t="n">
-        <v>42.0</v>
+        <v>0.0</v>
       </c>
       <c r="W79" t="n">
         <v>3.0</v>
@@ -8714,10 +8714,10 @@
         <v>0.0</v>
       </c>
       <c r="U80" t="n">
+        <v>166.0</v>
+      </c>
+      <c r="V80" t="n">
         <v>35.0</v>
-      </c>
-      <c r="V80" t="n">
-        <v>166.0</v>
       </c>
       <c r="W80" t="n">
         <v>3.0</v>
@@ -8922,10 +8922,10 @@
         <v>0.0</v>
       </c>
       <c r="U82" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="V82" t="n">
         <v>27.0</v>
-      </c>
-      <c r="V82" t="n">
-        <v>1.0</v>
       </c>
       <c r="W82" t="n">
         <v>1.0</v>
@@ -9026,10 +9026,10 @@
         <v>0.0</v>
       </c>
       <c r="U83" t="n">
+        <v>14.0</v>
+      </c>
+      <c r="V83" t="n">
         <v>36.0</v>
-      </c>
-      <c r="V83" t="n">
-        <v>14.0</v>
       </c>
       <c r="W83" t="n">
         <v>0.0</v>
@@ -9130,10 +9130,10 @@
         <v>0.0</v>
       </c>
       <c r="U84" t="n">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
       <c r="V84" t="n">
-        <v>2.0</v>
+        <v>0.0</v>
       </c>
       <c r="W84" t="n">
         <v>1.0</v>
@@ -9234,10 +9234,10 @@
         <v>0.0</v>
       </c>
       <c r="U85" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="V85" t="n">
         <v>14.0</v>
-      </c>
-      <c r="V85" t="n">
-        <v>3.0</v>
       </c>
       <c r="W85" t="n">
         <v>0.0</v>
@@ -9455,10 +9455,10 @@
         <v>0.0</v>
       </c>
       <c r="U2" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="V2" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="W2" t="n">
         <v>0.0</v>
@@ -9559,10 +9559,10 @@
         <v>0.0</v>
       </c>
       <c r="U3" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="V3" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="W3" t="n">
         <v>1.0</v>
@@ -9975,10 +9975,10 @@
         <v>0.0</v>
       </c>
       <c r="U7" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="V7" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="W7" t="n">
         <v>0.0</v>
@@ -10183,10 +10183,10 @@
         <v>0.0</v>
       </c>
       <c r="U9" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="V9" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="W9" t="n">
         <v>1.0</v>
@@ -10287,10 +10287,10 @@
         <v>0.0</v>
       </c>
       <c r="U10" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="V10" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="W10" t="n">
         <v>0.0</v>
@@ -10391,10 +10391,10 @@
         <v>0.0</v>
       </c>
       <c r="U11" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="V11" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="W11" t="n">
         <v>1.0</v>
@@ -10495,10 +10495,10 @@
         <v>0.0</v>
       </c>
       <c r="U12" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="V12" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="W12" t="n">
         <v>1.0</v>
@@ -10599,10 +10599,10 @@
         <v>0.0</v>
       </c>
       <c r="U13" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="V13" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="W13" t="n">
         <v>0.0</v>
@@ -10911,10 +10911,10 @@
         <v>0.0</v>
       </c>
       <c r="U16" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="V16" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="W16" t="n">
         <v>1.0</v>
@@ -11327,10 +11327,10 @@
         <v>0.0</v>
       </c>
       <c r="U20" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="V20" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="W20" t="n">
         <v>0.0</v>
@@ -11847,10 +11847,10 @@
         <v>0.0</v>
       </c>
       <c r="U25" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="V25" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="W25" t="n">
         <v>0.0</v>
@@ -11951,10 +11951,10 @@
         <v>0.0</v>
       </c>
       <c r="U26" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="V26" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="W26" t="n">
         <v>0.0</v>
@@ -12159,10 +12159,10 @@
         <v>0.0</v>
       </c>
       <c r="U28" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="V28" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="W28" t="n">
         <v>0.0</v>
@@ -12263,10 +12263,10 @@
         <v>0.0</v>
       </c>
       <c r="U29" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="V29" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="W29" t="n">
         <v>0.0</v>
@@ -12367,10 +12367,10 @@
         <v>0.0</v>
       </c>
       <c r="U30" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="V30" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="W30" t="n">
         <v>0.0</v>
@@ -12471,10 +12471,10 @@
         <v>0.0</v>
       </c>
       <c r="U31" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="V31" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="W31" t="n">
         <v>0.0</v>
@@ -12887,10 +12887,10 @@
         <v>0.0</v>
       </c>
       <c r="U35" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="V35" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="W35" t="n">
         <v>1.0</v>
@@ -13303,10 +13303,10 @@
         <v>0.0</v>
       </c>
       <c r="U39" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="V39" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="W39" t="n">
         <v>0.0</v>
@@ -13823,10 +13823,10 @@
         <v>0.0</v>
       </c>
       <c r="U44" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="V44" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="W44" t="n">
         <v>0.0</v>
@@ -14447,10 +14447,10 @@
         <v>0.0</v>
       </c>
       <c r="U50" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="V50" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="W50" t="n">
         <v>0.0</v>
@@ -14759,10 +14759,10 @@
         <v>0.0</v>
       </c>
       <c r="U53" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="V53" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="W53" t="n">
         <v>0.0</v>
@@ -14967,10 +14967,10 @@
         <v>0.0</v>
       </c>
       <c r="U55" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="V55" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="W55" t="n">
         <v>0.0</v>
@@ -15279,10 +15279,10 @@
         <v>0.0</v>
       </c>
       <c r="U58" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="V58" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="W58" t="n">
         <v>0.0</v>
@@ -15591,10 +15591,10 @@
         <v>0.0</v>
       </c>
       <c r="U61" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="V61" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="W61" t="n">
         <v>0.0</v>
@@ -15695,10 +15695,10 @@
         <v>0.0</v>
       </c>
       <c r="U62" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="V62" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="W62" t="n">
         <v>0.0</v>
@@ -15903,10 +15903,10 @@
         <v>0.0</v>
       </c>
       <c r="U64" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="V64" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="W64" t="n">
         <v>0.0</v>
@@ -16007,10 +16007,10 @@
         <v>0.0</v>
       </c>
       <c r="U65" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="V65" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="W65" t="n">
         <v>1.0</v>
@@ -16111,10 +16111,10 @@
         <v>0.0</v>
       </c>
       <c r="U66" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="V66" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="W66" t="n">
         <v>0.0</v>
@@ -16215,10 +16215,10 @@
         <v>0.0</v>
       </c>
       <c r="U67" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="V67" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="W67" t="n">
         <v>0.0</v>
@@ -16423,10 +16423,10 @@
         <v>0.0</v>
       </c>
       <c r="U69" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="V69" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="W69" t="n">
         <v>1.0</v>
@@ -16631,10 +16631,10 @@
         <v>0.0</v>
       </c>
       <c r="U71" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="V71" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="W71" t="n">
         <v>1.0</v>
@@ -16943,10 +16943,10 @@
         <v>0.0</v>
       </c>
       <c r="U74" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="V74" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="W74" t="n">
         <v>1.0</v>
@@ -17359,10 +17359,10 @@
         <v>0.0</v>
       </c>
       <c r="U78" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="V78" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="W78" t="n">
         <v>1.0</v>
@@ -17463,10 +17463,10 @@
         <v>0.0</v>
       </c>
       <c r="U79" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="V79" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="W79" t="n">
         <v>1.0</v>
@@ -17983,10 +17983,10 @@
         <v>0.0</v>
       </c>
       <c r="U84" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="V84" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="W84" t="n">
         <v>1.0</v>
@@ -18308,10 +18308,10 @@
         <v>0.0</v>
       </c>
       <c r="U2" t="n">
-        <v>0.0</v>
+        <v>0.05</v>
       </c>
       <c r="V2" t="n">
-        <v>0.05</v>
+        <v>0.0</v>
       </c>
       <c r="W2" t="n">
         <v>0.0</v>
@@ -18828,10 +18828,10 @@
         <v>0.0</v>
       </c>
       <c r="U7" t="n">
-        <v>0.0</v>
+        <v>0.1</v>
       </c>
       <c r="V7" t="n">
-        <v>0.1</v>
+        <v>0.0</v>
       </c>
       <c r="W7" t="n">
         <v>0.0</v>
@@ -19140,10 +19140,10 @@
         <v>0.0</v>
       </c>
       <c r="U10" t="n">
-        <v>0.0</v>
+        <v>0.04</v>
       </c>
       <c r="V10" t="n">
-        <v>0.04</v>
+        <v>0.0</v>
       </c>
       <c r="W10" t="n">
         <v>0.0</v>
@@ -20180,10 +20180,10 @@
         <v>0.0</v>
       </c>
       <c r="U20" t="n">
-        <v>0.0</v>
+        <v>0.06</v>
       </c>
       <c r="V20" t="n">
-        <v>0.06</v>
+        <v>0.0</v>
       </c>
       <c r="W20" t="n">
         <v>0.0</v>
@@ -20700,10 +20700,10 @@
         <v>0.0</v>
       </c>
       <c r="U25" t="n">
-        <v>0.0</v>
+        <v>0.01</v>
       </c>
       <c r="V25" t="n">
-        <v>0.01</v>
+        <v>0.0</v>
       </c>
       <c r="W25" t="n">
         <v>0.0</v>
@@ -20804,10 +20804,10 @@
         <v>0.0</v>
       </c>
       <c r="U26" t="n">
-        <v>0.0</v>
+        <v>0.02</v>
       </c>
       <c r="V26" t="n">
-        <v>0.02</v>
+        <v>0.0</v>
       </c>
       <c r="W26" t="n">
         <v>0.0</v>
@@ -21012,10 +21012,10 @@
         <v>0.0</v>
       </c>
       <c r="U28" t="n">
-        <v>0.0</v>
+        <v>0.01</v>
       </c>
       <c r="V28" t="n">
-        <v>0.01</v>
+        <v>0.0</v>
       </c>
       <c r="W28" t="n">
         <v>0.0</v>
@@ -21220,10 +21220,10 @@
         <v>0.0</v>
       </c>
       <c r="U30" t="n">
-        <v>0.0</v>
+        <v>0.01</v>
       </c>
       <c r="V30" t="n">
-        <v>0.01</v>
+        <v>0.0</v>
       </c>
       <c r="W30" t="n">
         <v>0.0</v>
@@ -21324,10 +21324,10 @@
         <v>0.0</v>
       </c>
       <c r="U31" t="n">
-        <v>0.0</v>
+        <v>0.01</v>
       </c>
       <c r="V31" t="n">
-        <v>0.01</v>
+        <v>0.0</v>
       </c>
       <c r="W31" t="n">
         <v>0.0</v>
@@ -21740,10 +21740,10 @@
         <v>0.0</v>
       </c>
       <c r="U35" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="V35" t="n">
         <v>0.01</v>
-      </c>
-      <c r="V35" t="n">
-        <v>0.0</v>
       </c>
       <c r="W35" t="n">
         <v>0.0</v>
@@ -22780,10 +22780,10 @@
         <v>0.0</v>
       </c>
       <c r="U45" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="V45" t="n">
         <v>0.01</v>
-      </c>
-      <c r="V45" t="n">
-        <v>0.0</v>
       </c>
       <c r="W45" t="n">
         <v>0.0</v>
@@ -23820,10 +23820,10 @@
         <v>0.0</v>
       </c>
       <c r="U55" t="n">
-        <v>0.0</v>
+        <v>0.01</v>
       </c>
       <c r="V55" t="n">
-        <v>0.01</v>
+        <v>0.0</v>
       </c>
       <c r="W55" t="n">
         <v>0.0</v>
@@ -24444,10 +24444,10 @@
         <v>0.0</v>
       </c>
       <c r="U61" t="n">
-        <v>0.0</v>
+        <v>0.01</v>
       </c>
       <c r="V61" t="n">
-        <v>0.01</v>
+        <v>0.0</v>
       </c>
       <c r="W61" t="n">
         <v>0.0</v>
@@ -24548,10 +24548,10 @@
         <v>0.0</v>
       </c>
       <c r="U62" t="n">
-        <v>0.0</v>
+        <v>0.01</v>
       </c>
       <c r="V62" t="n">
-        <v>0.01</v>
+        <v>0.0</v>
       </c>
       <c r="W62" t="n">
         <v>0.0</v>
@@ -24756,10 +24756,10 @@
         <v>0.0</v>
       </c>
       <c r="U64" t="n">
-        <v>0.0</v>
+        <v>0.01</v>
       </c>
       <c r="V64" t="n">
-        <v>0.01</v>
+        <v>0.0</v>
       </c>
       <c r="W64" t="n">
         <v>0.0</v>
@@ -24860,10 +24860,10 @@
         <v>0.0</v>
       </c>
       <c r="U65" t="n">
-        <v>0.0</v>
+        <v>0.01</v>
       </c>
       <c r="V65" t="n">
-        <v>0.01</v>
+        <v>0.0</v>
       </c>
       <c r="W65" t="n">
         <v>0.0</v>
@@ -24964,10 +24964,10 @@
         <v>0.0</v>
       </c>
       <c r="U66" t="n">
-        <v>0.0</v>
+        <v>0.01</v>
       </c>
       <c r="V66" t="n">
-        <v>0.01</v>
+        <v>0.0</v>
       </c>
       <c r="W66" t="n">
         <v>0.0</v>
@@ -25068,10 +25068,10 @@
         <v>0.0</v>
       </c>
       <c r="U67" t="n">
-        <v>0.0</v>
+        <v>0.01</v>
       </c>
       <c r="V67" t="n">
-        <v>0.01</v>
+        <v>0.0</v>
       </c>
       <c r="W67" t="n">
         <v>0.0</v>
@@ -25276,10 +25276,10 @@
         <v>0.0</v>
       </c>
       <c r="U69" t="n">
-        <v>0.0</v>
+        <v>0.01</v>
       </c>
       <c r="V69" t="n">
-        <v>0.01</v>
+        <v>0.0</v>
       </c>
       <c r="W69" t="n">
         <v>0.0</v>
@@ -25484,10 +25484,10 @@
         <v>0.0</v>
       </c>
       <c r="U71" t="n">
-        <v>0.0</v>
+        <v>0.03</v>
       </c>
       <c r="V71" t="n">
-        <v>0.03</v>
+        <v>0.0</v>
       </c>
       <c r="W71" t="n">
         <v>0.0</v>
@@ -26004,10 +26004,10 @@
         <v>0.0</v>
       </c>
       <c r="U76" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="V76" t="n">
         <v>0.01</v>
-      </c>
-      <c r="V76" t="n">
-        <v>0.0</v>
       </c>
       <c r="W76" t="n">
         <v>0.0</v>
@@ -26212,10 +26212,10 @@
         <v>0.0</v>
       </c>
       <c r="U78" t="n">
-        <v>0.0</v>
+        <v>0.01</v>
       </c>
       <c r="V78" t="n">
-        <v>0.01</v>
+        <v>0.0</v>
       </c>
       <c r="W78" t="n">
         <v>0.0</v>
@@ -26316,10 +26316,10 @@
         <v>0.0</v>
       </c>
       <c r="U79" t="n">
-        <v>0.0</v>
+        <v>0.01</v>
       </c>
       <c r="V79" t="n">
-        <v>0.01</v>
+        <v>0.0</v>
       </c>
       <c r="W79" t="n">
         <v>0.0</v>
@@ -26420,10 +26420,10 @@
         <v>0.0</v>
       </c>
       <c r="U80" t="n">
-        <v>0.0</v>
+        <v>0.02</v>
       </c>
       <c r="V80" t="n">
-        <v>0.02</v>
+        <v>0.0</v>
       </c>
       <c r="W80" t="n">
         <v>0.0</v>
@@ -26628,10 +26628,10 @@
         <v>0.0</v>
       </c>
       <c r="U82" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="V82" t="n">
         <v>0.01</v>
-      </c>
-      <c r="V82" t="n">
-        <v>0.0</v>
       </c>
       <c r="W82" t="n">
         <v>0.0</v>
@@ -26732,10 +26732,10 @@
         <v>0.0</v>
       </c>
       <c r="U83" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="V83" t="n">
         <v>0.02</v>
-      </c>
-      <c r="V83" t="n">
-        <v>0.01</v>
       </c>
       <c r="W83" t="n">
         <v>0.0</v>
@@ -26940,10 +26940,10 @@
         <v>0.0</v>
       </c>
       <c r="U85" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="V85" t="n">
         <v>0.01</v>
-      </c>
-      <c r="V85" t="n">
-        <v>0.0</v>
       </c>
       <c r="W85" t="n">
         <v>0.0</v>

</xml_diff>